<commit_message>
Larson recommended changes to Model dev calendar
</commit_message>
<xml_diff>
--- a/ProjectTimeline.xlsx
+++ b/ProjectTimeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Domain Knowledge Research</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>Poster Printing/Shipping</t>
+  </si>
+  <si>
+    <t>Binary Sidewalk detector, investigate convolutional architectures for automatically labeling sidewalks in images (10 days)</t>
+  </si>
+  <si>
+    <t>Sidewalk quality detection, adapt architectures for detection and quality classification</t>
+  </si>
+  <si>
+    <t>Parameters tuning and further architecture exploration</t>
+  </si>
+  <si>
+    <t>Evaluation of models to other neighborhoods</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Identification of individual labels that contribute to overall rating</t>
   </si>
 </sst>
 </file>
@@ -221,9 +236,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$28</c:f>
+              <c:f>Sheet1!$A$2:$B$32</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="31"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Understand Social and Public Health considerations of sidewalks</c:v>
@@ -264,28 +279,43 @@
                   <c:pt idx="14">
                     <c:v>Development of Machine Learning/Neural Network, Cross Validation, Testing</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Binary Sidewalk detector, investigate convolutional architectures for automatically labeling sidewalks in images (10 days)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Sidewalk quality detection, adapt architectures for detection and quality classification</c:v>
+                  </c:pt>
                   <c:pt idx="17">
+                    <c:v>Parameters tuning and further architecture exploration</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Evaluation of models to other neighborhoods</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v> Identification of individual labels that contribute to overall rating</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>Written Paper - 1st Draft</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="22">
                     <c:v>Poster Creation</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="23">
                     <c:v>Poster Printing/Shipping</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="26">
                     <c:v>Problem Proposal</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="27">
                     <c:v>Café Talk I</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="28">
                     <c:v>First Paper Draft Due</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="29">
                     <c:v>Café Talk II</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="30">
                     <c:v>Final Poster Presentation</c:v>
                   </c:pt>
                 </c:lvl>
@@ -302,10 +332,10 @@
                   <c:pt idx="13">
                     <c:v>Model Development</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="20">
                     <c:v>Documentation</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="25">
                     <c:v>Presentation/Review Steps</c:v>
                   </c:pt>
                 </c:lvl>
@@ -314,10 +344,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$28</c:f>
+              <c:f>Sheet1!$C$2:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>42879</c:v>
                 </c:pt>
@@ -354,28 +384,43 @@
                 <c:pt idx="14">
                   <c:v>42901</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>42903</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42911</c:v>
+                </c:pt>
                 <c:pt idx="17">
+                  <c:v>42921</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42931</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42941</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>42887</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="22">
                   <c:v>42979</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="23">
                   <c:v>43024</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>42879</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>42892</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
                   <c:v>42921</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="29">
                   <c:v>42927</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="30">
                   <c:v>43048</c:v>
                 </c:pt>
               </c:numCache>
@@ -408,9 +453,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$28</c:f>
+              <c:f>Sheet1!$A$2:$B$32</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="31"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Understand Social and Public Health considerations of sidewalks</c:v>
@@ -451,28 +496,43 @@
                   <c:pt idx="14">
                     <c:v>Development of Machine Learning/Neural Network, Cross Validation, Testing</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Binary Sidewalk detector, investigate convolutional architectures for automatically labeling sidewalks in images (10 days)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Sidewalk quality detection, adapt architectures for detection and quality classification</c:v>
+                  </c:pt>
                   <c:pt idx="17">
+                    <c:v>Parameters tuning and further architecture exploration</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Evaluation of models to other neighborhoods</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v> Identification of individual labels that contribute to overall rating</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>Written Paper - 1st Draft</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="22">
                     <c:v>Poster Creation</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="23">
                     <c:v>Poster Printing/Shipping</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="26">
                     <c:v>Problem Proposal</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="27">
                     <c:v>Café Talk I</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="28">
                     <c:v>First Paper Draft Due</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="29">
                     <c:v>Café Talk II</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="30">
                     <c:v>Final Poster Presentation</c:v>
                   </c:pt>
                 </c:lvl>
@@ -489,10 +549,10 @@
                   <c:pt idx="13">
                     <c:v>Model Development</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="20">
                     <c:v>Documentation</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="25">
                     <c:v>Presentation/Review Steps</c:v>
                   </c:pt>
                 </c:lvl>
@@ -501,10 +561,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$28</c:f>
+              <c:f>Sheet1!$D$2:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -541,28 +601,43 @@
                 <c:pt idx="14">
                   <c:v>75</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
                 <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="22">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="23">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="29">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -579,11 +654,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="624443184"/>
-        <c:axId val="624442792"/>
+        <c:axId val="700421648"/>
+        <c:axId val="700422040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624443184"/>
+        <c:axId val="700421648"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -626,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624442792"/>
+        <c:crossAx val="700422040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -634,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624442792"/>
+        <c:axId val="700422040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42879"/>
@@ -686,7 +761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624443184"/>
+        <c:crossAx val="700421648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1289,14 +1364,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1581,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1695,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E27" si="0">C2+D2</f>
+        <f t="shared" ref="E2:E31" si="0">C2+D2</f>
         <v>42899</v>
       </c>
       <c r="G2" s="3">
@@ -1658,7 +1733,7 @@
         <v>42899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1816,148 +1891,224 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2">
+        <v>42903</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>42913</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>42911</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>42926</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" t="s">
-        <v>21</v>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="2">
-        <v>42887</v>
+        <v>42921</v>
       </c>
       <c r="D19">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>42921</v>
+        <v>42936</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" t="s">
-        <v>27</v>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C20" s="2">
-        <v>42979</v>
+        <v>42931</v>
       </c>
       <c r="D20">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>43024</v>
+        <v>42941</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" t="s">
-        <v>28</v>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="2">
-        <f>E20</f>
-        <v>43024</v>
+        <v>42941</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>43034</v>
+        <v>42961</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>16</v>
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2">
+        <v>42887</v>
+      </c>
+      <c r="D23">
+        <v>34</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>42921</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2">
-        <v>42879</v>
+        <v>42979</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>42886</v>
+        <v>43024</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2">
-        <v>42892</v>
+        <f>E24</f>
+        <v>43024</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>42893</v>
+        <v>43034</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2">
+        <v>42879</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>42886</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2">
+        <v>42892</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>42893</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C30" s="2">
         <v>42921</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>1</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E30" s="2">
         <f t="shared" si="0"/>
         <v>42922</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C31" s="2">
         <v>42927</v>
       </c>
-      <c r="D27">
+      <c r="D31">
         <v>1</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E31" s="2">
         <f t="shared" si="0"/>
         <v>42928</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C32" s="2">
         <v>43048</v>
       </c>
-      <c r="D28">
+      <c r="D32">
         <v>1</v>
       </c>
-      <c r="E28" s="2">
-        <f>C28+D28</f>
+      <c r="E32" s="2">
+        <f>C32+D32</f>
         <v>43049</v>
       </c>
     </row>

</xml_diff>